<commit_message>
Agregar notas excel, modificaciones en prioridades y stack, no funcional el guardado en archivo y eliminación de tareas
</commit_message>
<xml_diff>
--- a/Recursos/Tareas.xlsx
+++ b/Recursos/Tareas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Programa</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Núcleo</t>
   </si>
   <si>
-    <t xml:space="preserve">No configurado</t>
-  </si>
-  <si>
     <t>Prioridad</t>
   </si>
   <si>
@@ -84,9 +81,21 @@
     <t xml:space="preserve">TI + 2</t>
   </si>
   <si>
+    <t>TI+6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI + 5</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Tamaño</t>
   </si>
   <si>
+    <t>Ver</t>
+  </si>
+  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -112,6 +121,15 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3584 timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timer task solo en cpu0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambiar nivel de interrupción de timer a 2 mejora los errores</t>
   </si>
 </sst>
 </file>
@@ -126,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +181,12 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -467,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -558,6 +582,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -1071,7 +1104,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1160,211 +1193,232 @@
         <v>16</v>
       </c>
       <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20">
         <v>1</v>
-      </c>
-      <c r="C4" s="20">
-        <v>1</v>
-      </c>
-      <c r="D4" s="20">
-        <v>0</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
       </c>
       <c r="F4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="19">
         <v>0</v>
       </c>
       <c r="H4" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="21">
         <v>0</v>
       </c>
       <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1</v>
       </c>
       <c r="L4" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="D5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="E5" s="24" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>22</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="8">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="27">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C6" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D6" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E6" s="29">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F6" s="30">
-        <v>10</v>
-      </c>
-      <c r="G6" s="27">
+        <v>2</v>
+      </c>
+      <c r="G6" s="31">
         <v>5</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="32">
         <v>5</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="33">
         <v>5</v>
       </c>
       <c r="J6" s="26">
-        <v>2048</v>
+        <v>2</v>
       </c>
       <c r="K6" s="27">
         <f>5*4096</f>
         <v>20480</v>
       </c>
       <c r="L6" s="29">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="J7" s="31"/>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1536</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="20">
-        <v>1536</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="23"/>
+      <c r="A13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="20">
+        <f>J6+K6</f>
+        <v>20482</v>
+      </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="20">
-        <f>J6+K6</f>
-        <v>22528</v>
+        <f>(B6+C6+D6+E6+F6+G6+H6+I6+L6)*B9</f>
+        <v>43008</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B15" s="20">
-        <f>(B6+C6+D6+E6+F6+G6+H6+I6+L6)*B10</f>
-        <v>107520</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="20">
-        <f>B14+B15</f>
-        <v>130048</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25"/>
+        <f>B13+B14</f>
+        <v>63490</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25"/>
+    <row r="17" ht="14.25">
+      <c r="A17" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>32</v>
+      <c r="A18" s="20">
+        <v>0</v>
+      </c>
+      <c r="B18" s="20">
+        <f>COUNTIF($B$4:$L$4,0)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="20">
-        <f>COUNTIF($B$4:$L$4,0)</f>
+        <f>COUNTIF($B$4:$L$4,1)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="20">
-        <f>COUNTIF($B$4:$L$4,1)</f>
-        <v>4</v>
-      </c>
-    </row>
+    <row r="20" ht="14.25"/>
     <row r="21" ht="14.25"/>
+    <row r="22" ht="14.25">
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Agregar codigo peltier a hornito-espA
</commit_message>
<xml_diff>
--- a/Recursos/Tareas.xlsx
+++ b/Recursos/Tareas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Programa</t>
   </si>
@@ -33,6 +33,12 @@
     <t>webserver.c</t>
   </si>
   <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
     <t>Tarea</t>
   </si>
   <si>
@@ -63,9 +69,21 @@
     <t xml:space="preserve">Actualización de datos</t>
   </si>
   <si>
+    <t xml:space="preserve">Muestreo señal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_0 (GPIO 36)</t>
+  </si>
+  <si>
     <t>Núcleo</t>
   </si>
   <si>
+    <t xml:space="preserve">NTC Placa caliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_3 (GPIO 39)</t>
+  </si>
+  <si>
     <t>Prioridad</t>
   </si>
   <si>
@@ -90,6 +108,9 @@
     <t>?</t>
   </si>
   <si>
+    <t xml:space="preserve">NTC Placa fría</t>
+  </si>
+  <si>
     <t>Tamaño</t>
   </si>
   <si>
@@ -130,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cambiar nivel de interrupción de timer a 2 mejora los errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestreo V</t>
   </si>
 </sst>
 </file>
@@ -491,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -549,9 +573,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1089,13 +1110,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="9.08203125"/>
+    <col customWidth="1" min="1" max="1" width="15.28125"/>
     <col customWidth="1" min="2" max="2" width="9.140625"/>
     <col customWidth="1" min="3" max="3" width="12.8515625"/>
     <col customWidth="1" min="4" max="4" width="18.28125"/>
@@ -1107,6 +1128,8 @@
     <col customWidth="1" min="10" max="10" width="10.140625"/>
     <col customWidth="1" min="11" max="11" width="14.7109375"/>
     <col customWidth="1" min="12" max="12" width="21.57421875"/>
+    <col customWidth="1" min="14" max="14" width="17.28125"/>
+    <col customWidth="1" min="15" max="15" width="17.8515625"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.25">
@@ -1134,48 +1157,60 @@
         <v>5</v>
       </c>
       <c r="L2" s="4"/>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="J3" s="15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" s="18">
         <v>0</v>
@@ -1210,101 +1245,110 @@
       <c r="L4" s="20">
         <v>1</v>
       </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="23">
+      <c r="A6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="22">
         <v>2</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>2</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>2</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>2</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>5</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <v>5</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="27">
         <v>5</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="21">
         <v>2</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="22">
         <f>5*4096</f>
         <v>20480</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="24">
         <v>3</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="29"/>
+        <v>33</v>
+      </c>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="19" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B9" s="19">
         <v>1536</v>
@@ -1312,24 +1356,24 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="19" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B12" s="19"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="19" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B13" s="19">
         <f>J6+K6</f>
@@ -1338,7 +1382,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" s="19">
         <f>(B6+C6+D6+E6+F6+G6+H6+I6+L6)*B9</f>
@@ -1347,7 +1391,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="19" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B15" s="19">
         <f>B13+B14</f>
@@ -1357,10 +1401,10 @@
     <row r="16" ht="14.25"/>
     <row r="17" ht="14.25">
       <c r="A17" s="19" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" ht="14.25">
@@ -1385,17 +1429,30 @@
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar excel con datos actuales
</commit_message>
<xml_diff>
--- a/Recursos/Tareas.xlsx
+++ b/Recursos/Tareas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Programa</t>
   </si>
@@ -111,27 +111,60 @@
     <t xml:space="preserve">NTC Placa fría</t>
   </si>
   <si>
+    <t xml:space="preserve">ADC1_6 (GPIO 34)</t>
+  </si>
+  <si>
     <t>Tamaño</t>
   </si>
   <si>
+    <t xml:space="preserve">Cruce por cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO 26</t>
+  </si>
+  <si>
     <t>Ver</t>
   </si>
   <si>
+    <t xml:space="preserve">Salida Dimmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO 27</t>
+  </si>
+  <si>
     <t>Variables</t>
   </si>
   <si>
     <t>Valor</t>
   </si>
   <si>
+    <t xml:space="preserve">Peltier 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO 32</t>
+  </si>
+  <si>
     <t>CM</t>
   </si>
   <si>
+    <t xml:space="preserve">Peltier 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO 33</t>
+  </si>
+  <si>
     <t>TI</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
+    <t>Bomba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO 25</t>
+  </si>
+  <si>
     <t>Bytes</t>
   </si>
   <si>
@@ -151,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cambiar nivel de interrupción de timer a 2 mejora los errores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muestreo V</t>
   </si>
 </sst>
 </file>
@@ -168,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,14 +235,8 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor rgb="FF0070C0"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -511,11 +535,24 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,6 +606,9 @@
     <xf fontId="0" fillId="4" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,16 +630,10 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="7" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1116,7 +1150,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.28125"/>
+    <col customWidth="1" min="1" max="1" width="10.7109375"/>
     <col customWidth="1" min="2" max="2" width="9.140625"/>
     <col customWidth="1" min="3" max="3" width="12.8515625"/>
     <col customWidth="1" min="4" max="4" width="18.28125"/>
@@ -1157,10 +1191,10 @@
         <v>5</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1201,10 +1235,10 @@
       <c r="L3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1212,43 +1246,43 @@
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="19">
         <v>0</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="20">
         <v>1</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="19">
         <v>0</v>
       </c>
-      <c r="G4" s="18">
+      <c r="H4" s="20">
+        <v>1</v>
+      </c>
+      <c r="I4" s="21">
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="19">
         <v>1</v>
       </c>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="L4" s="21">
         <v>1</v>
       </c>
-      <c r="K4" s="18">
-        <v>1</v>
-      </c>
-      <c r="L4" s="20">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1256,205 +1290,227 @@
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="O5" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="22">
-        <v>2</v>
-      </c>
-      <c r="C6" s="23">
-        <v>2</v>
-      </c>
-      <c r="D6" s="23">
-        <v>2</v>
-      </c>
-      <c r="E6" s="24">
-        <v>2</v>
-      </c>
-      <c r="F6" s="21">
-        <v>2</v>
-      </c>
-      <c r="G6" s="25">
+      <c r="A6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="23">
         <v>5</v>
       </c>
-      <c r="H6" s="26">
+      <c r="C6" s="24">
         <v>5</v>
       </c>
-      <c r="I6" s="27">
+      <c r="D6" s="24">
         <v>5</v>
       </c>
-      <c r="J6" s="21">
-        <v>2</v>
-      </c>
-      <c r="K6" s="22">
+      <c r="E6" s="25">
+        <v>5</v>
+      </c>
+      <c r="F6" s="22">
+        <v>5</v>
+      </c>
+      <c r="G6" s="23">
+        <v>5</v>
+      </c>
+      <c r="H6" s="24">
+        <v>5</v>
+      </c>
+      <c r="I6" s="25">
+        <v>5</v>
+      </c>
+      <c r="J6" s="22">
+        <v>5</v>
+      </c>
+      <c r="K6" s="23">
         <f>5*4096</f>
         <v>20480</v>
       </c>
-      <c r="L6" s="24">
-        <v>3</v>
+      <c r="L6" s="25">
+        <v>5</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="N7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1536</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="19">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="D11" s="29"/>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="19">
+      <c r="A13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="20">
         <f>J6+K6</f>
-        <v>20482</v>
+        <v>20485</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="19">
+      <c r="A14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="20">
         <f>(B6+C6+D6+E6+F6+G6+H6+I6+L6)*B9</f>
-        <v>43008</v>
+        <v>69120</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="19">
+      <c r="A15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="20">
         <f>B13+B14</f>
-        <v>63490</v>
+        <v>89605</v>
       </c>
     </row>
     <row r="16" ht="14.25"/>
     <row r="17" ht="14.25">
-      <c r="A17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>42</v>
+      <c r="A17" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="19">
+      <c r="A18" s="20">
         <v>0</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="20">
         <f>COUNTIF($B$4:$L$4,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="20">
+        <v>1</v>
+      </c>
+      <c r="B19" s="20">
+        <f>COUNTIF($B$4:$L$4,1)</f>
         <v>5</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="19">
-        <f>COUNTIF($B$4:$L$4,1)</f>
-        <v>6</v>
       </c>
     </row>
     <row r="20" ht="14.25"/>
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25">
       <c r="B22" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="B24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25"/>
+    <row r="29" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Modificacion sistema de control y tiempos
</commit_message>
<xml_diff>
--- a/Recursos/Tareas.xlsx
+++ b/Recursos/Tareas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Programa</t>
   </si>
@@ -177,13 +177,16 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t xml:space="preserve">3584 timer</t>
+    <t xml:space="preserve">Timer 5500</t>
   </si>
   <si>
     <t xml:space="preserve">timer task solo en cpu0</t>
   </si>
   <si>
     <t xml:space="preserve">Cambiar nivel de interrupción de timer a 2 mejora los errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wifi en cpu1</t>
   </si>
 </sst>
 </file>
@@ -1509,6 +1512,11 @@
         <v>56</v>
       </c>
     </row>
+    <row r="25" ht="14.25">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="28" ht="14.25"/>
     <row r="29" ht="14.25"/>
   </sheetData>

</xml_diff>